<commit_message>
7/11/18 - Joanna's latest code
Includes definition of delta and SN_length in species functions file. Adds lines to PERTspecies.R to change to the current working directory. Changes CR_KR_ONE.R to calculate functional KR (using delta as a weight).
</commit_message>
<xml_diff>
--- a/CodeMonarchs_NewEqn/Baseline1/network_inputs_monarch.xlsx
+++ b/CodeMonarchs_NewEqn/Baseline1/network_inputs_monarch.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Pop" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,44 +18,57 @@
     <sheet name="September" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="21">
   <si>
-    <t>Node</t>
+    <t xml:space="preserve">Node</t>
   </si>
   <si>
-    <t>N0 - initial population at start of winter</t>
+    <t xml:space="preserve">N0 - initial population at start of winter</t>
   </si>
   <si>
-    <t>W</t>
+    <t xml:space="preserve">W</t>
   </si>
   <si>
-    <t>S</t>
+    <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t>C</t>
+    <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t>N</t>
+    <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t>Node attributes ALPHA</t>
+    <t xml:space="preserve">Node attributes ALPHA</t>
   </si>
   <si>
-    <t>Adult survival</t>
+    <t xml:space="preserve">Adult survival</t>
   </si>
   <si>
-    <t>Pupal survival</t>
+    <t xml:space="preserve">Pupal survival</t>
   </si>
   <si>
-    <t># milkweed in node</t>
+    <t xml:space="preserve"># milkweed in node</t>
   </si>
   <si>
     <r>
-      <t>Tell code to </t>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tell code to </t>
     </r>
     <r>
       <rPr>
@@ -67,38 +80,38 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>STOP</t>
+      <t xml:space="preserve">STOP</t>
     </r>
   </si>
   <si>
-    <t>NOTES:</t>
+    <t xml:space="preserve">NOTES:</t>
   </si>
   <si>
-    <t>Variable Names</t>
+    <t xml:space="preserve">Variable Names</t>
   </si>
   <si>
-    <t>sA</t>
+    <t xml:space="preserve">sA</t>
   </si>
   <si>
-    <t>sP</t>
+    <t xml:space="preserve">sP</t>
   </si>
   <si>
-    <t>m</t>
+    <t xml:space="preserve">m</t>
   </si>
   <si>
-    <t>STOP</t>
+    <t xml:space="preserve">STOP</t>
   </si>
   <si>
-    <t>Destination</t>
+    <t xml:space="preserve">Destination</t>
   </si>
   <si>
-    <t>Transitions pij</t>
+    <t xml:space="preserve">Transitions pij</t>
   </si>
   <si>
-    <t>Origin</t>
+    <t xml:space="preserve">Origin</t>
   </si>
   <si>
-    <t>Edge survival sij</t>
+    <t xml:space="preserve">Edge survival sij</t>
   </si>
 </sst>
 </file>
@@ -106,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
   <fonts count="11">
@@ -410,9 +423,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>586800</xdr:colOff>
+      <xdr:colOff>586440</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -421,8 +434,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7533720" y="0"/>
-          <a:ext cx="3949560" cy="2019240"/>
+          <a:off x="5981040" y="0"/>
+          <a:ext cx="3092040" cy="2018880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -455,9 +468,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>434520</xdr:colOff>
+      <xdr:colOff>434160</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:rowOff>183600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -466,8 +479,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7978680" y="801000"/>
-          <a:ext cx="3352320" cy="876240"/>
+          <a:off x="6254640" y="801000"/>
+          <a:ext cx="2666160" cy="875880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -492,27 +505,57 @@
         <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Parameters derived from Flockhart et al. (2015).</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Winter adult survival- 0.9896/month. This estimate excludes catastrophic events.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -532,9 +575,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -543,8 +586,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7949880" y="791280"/>
-          <a:ext cx="3961800" cy="1723320"/>
+          <a:off x="6225840" y="791280"/>
+          <a:ext cx="3103920" cy="1722960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -574,15 +617,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Parameters derived from Flockhart et al. (2015). Adult survival nonwinter breeding equation is exp(-days/25.5), line 216. We assume each month is 30 days.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -591,15 +649,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>#milkweed in node is derived from Table 1.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -607,7 +680,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -616,15 +699,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Edge transitions are derived from Table S3, p47</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -633,15 +731,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Migration survival derived from Table S4, p48</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -649,7 +762,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -669,9 +792,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -680,8 +803,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7949880" y="791280"/>
-          <a:ext cx="3961800" cy="1723320"/>
+          <a:off x="6225840" y="791280"/>
+          <a:ext cx="3103920" cy="1722960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -711,15 +834,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Parameters derived from Flockhart et al. (2015). Adult survival nonwinter breeding equation is exp(-days/25.5), line 216. We assume each month is 30 days.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -728,15 +866,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>#milkweed in node is derived from Table 1.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -744,7 +897,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -753,15 +916,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Edge transitions are derived from Table S3, p47</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -770,15 +948,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Migration survival derived from Table S4, p48</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -786,7 +979,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -806,9 +1009,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -817,8 +1020,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7949880" y="791280"/>
-          <a:ext cx="3961800" cy="1723320"/>
+          <a:off x="6225840" y="791280"/>
+          <a:ext cx="3103920" cy="1722960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -848,15 +1051,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Parameters derived from Flockhart et al. (2015). Adult survival nonwinter breeding equation is exp(-days/25.5), line 216. We assume each month is 30 days.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -865,15 +1083,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>#milkweed in node is derived from Table 1.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -881,7 +1114,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -890,15 +1133,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Edge transitions are derived from Table S3, p47</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -907,15 +1165,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Migration survival derived from Table S4, p48</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -923,7 +1196,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -943,9 +1226,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -954,8 +1237,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7949880" y="791280"/>
-          <a:ext cx="3961800" cy="1723320"/>
+          <a:off x="6225840" y="791280"/>
+          <a:ext cx="3103920" cy="1722960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -985,15 +1268,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Parameters derived from Flockhart et al. (2015). Adult survival nonwinter breeding equation is exp(-days/25.5), line 216. We assume each month is 30 days.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1002,15 +1300,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>#milkweed in node is derived from Table 1.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1018,7 +1331,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1027,15 +1350,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Edge transitions are derived from Table S3, p47</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1044,15 +1382,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Migration survival derived from Table S4, p48</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1060,7 +1413,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1080,9 +1443,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1091,8 +1454,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7949880" y="791280"/>
-          <a:ext cx="3961800" cy="1723320"/>
+          <a:off x="6225840" y="791280"/>
+          <a:ext cx="3103920" cy="1722960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1122,15 +1485,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Parameters derived from Flockhart et al. (2015). Adult survival nonwinter breeding equation is exp(-days/25.5), line 216. We assume each month is 30 days.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1139,15 +1517,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>#milkweed in node is derived from Table 1.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1155,7 +1548,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1164,15 +1567,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Edge transitions are derived from Table S3, p47</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1181,15 +1599,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Migration survival derived from Table S4, p48</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1197,7 +1630,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1217,9 +1660,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1228,8 +1671,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7949880" y="791280"/>
-          <a:ext cx="3961800" cy="1723320"/>
+          <a:off x="6225840" y="791280"/>
+          <a:ext cx="3103920" cy="1722960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1259,15 +1702,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Parameters derived from Flockhart et al. (2015). Adult survival nonwinter breeding equation is exp(-days/25.5), line 216. We assume each month is 30 days.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1276,15 +1734,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>#milkweed in node is derived from Table 1.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1292,7 +1765,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1301,15 +1784,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Edge transitions are derived from Table S3, p47</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1318,15 +1816,30 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
             <a:t>Migration survival derived from Table S4, p48</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr>
@@ -1334,7 +1847,17 @@
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1351,14 +1874,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="C3 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,16 +1942,16 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1452,7 +1975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1470,7 +1993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -1780,15 +2303,15 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="C3 A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2142,15 +2665,15 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="C3 A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2503,16 +3026,16 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="C3 A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2865,16 +3388,16 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="C3 A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3227,16 +3750,16 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="C3 A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3589,16 +4112,16 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="C3 A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>